<commit_message>
National_Parks_seeds.rb added but not yet migrated - commit done
</commit_message>
<xml_diff>
--- a/National Parks listed by state.xlsx
+++ b/National Parks listed by state.xlsx
@@ -21,17 +21,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="193">
   <si>
     <t xml:space="preserve">https://support.microsoft.com/en-us/office/concat-function-9b1a9a3f-94ff-41af-9736-694cbd6b4ca2</t>
   </si>
   <si>
+    <t xml:space="preserve">LISTING FROM CHATGPT OF HOW TO WRITE SEEDS.RB FILE</t>
+  </si>
+  <si>
     <t xml:space="preserve">National Park Name</t>
   </si>
   <si>
     <t xml:space="preserve">State(s)</t>
   </si>
   <si>
+    <t xml:space="preserve">CONCATANETE FORMULA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNFORMATTED COPY OF CONCATANETED COLUMN</t>
+  </si>
+  <si>
     <t xml:space="preserve">parks = [</t>
   </si>
   <si>
@@ -284,280 +293,313 @@
     <t xml:space="preserve"> { name: 'Great Sand Dunes National Park and Preserve', state: 'Colorado' },</t>
   </si>
   <si>
+    <t xml:space="preserve">Great Smoky Mountains National Park NC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Carolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Great Smoky Mountains National Park NC', state: 'North Carolina' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Smoky Mountains National Park TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennessee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Great Smoky Mountains National Park TN', state: 'Tennessee' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guadalupe Mountains National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Guadalupe Mountains National Park', state: 'Texas' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haleakalā National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Haleakalā National Park', state: 'Hawaii' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawai'i Volcanoes National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Hawaii Volcanoes National Park', state: 'Hawaii' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot Springs National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkansas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Hot Springs National Park', state: 'Arkansas' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiana Dunes National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Indiana Dunes National Park', state: 'Indiana' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isle Royale National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Isle Royale National Park', state: 'Michigan' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Tree National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Joshua Tree National Park', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katmai National Park and Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Katmai National Park and Preserve', state: 'Alaska' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenai Fjords National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Kenai Fjords National Park', state: 'Alaska' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kings Canyon National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Kings Canyon National Park', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kobuk Valley National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Kobuk Valley National Park', state: 'Alaska' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lake Clark National Park and Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Lake Clark National Park and Preserve', state: 'Alaska' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lassen Volcanic National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Lassen Volcanic National Park', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mammoth Cave National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kentucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Mammoth Cave National Park', state: 'Kentucky' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesa Verde National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Mesa Verde National Park', state: 'Colorado' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mount Rainier National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Mount Rainier National Park', state: 'Washington' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Cascades National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'North Cascades National Park', state: 'Washington' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olympic National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Olympic National Park', state: 'Washington' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrified Forest National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Petrified Forest National Park', state: 'Arizona' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinnacles National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Pinnacles National Park', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redwood National and State Parks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Redwood National and State Parks', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocky Mountain National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Rocky Mountain National Park', state: 'Colorado' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saguaro National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Saguaro National Park', state: 'Arizona' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequoia National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Sequoia National Park', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shenandoah National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Shenandoah National Park', state: 'Virginia' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theodore Roosevelt National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Dakota</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Theodore Roosevelt National Park', state: 'North Dakota' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virgin Islands National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U.S. Virgin Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Virgin Islands National Park', state: 'U.S. Virgin Islands' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voyageurs National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minnesota</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Voyageurs National Park', state: 'Minnesota' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Cave National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Wind Cave National Park', state: 'South Dakota' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrangell–St. Elias National Park and Preserve</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Wrangell–St. Elias National Park and Preserve', state: 'Alaska' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellowstone National Park ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idaho</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Yellowstone National Park ID', state: 'Idaho' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellowstone National Park MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Yellowstone National Park MT', state: 'Montana' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellowstone National Park WY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Yellowstone National Park WY', state: 'Wyoming' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yosemite National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Yosemite National Park', state: 'California' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zion National Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { name: 'Zion National Park', state: 'Utah' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that some national parks span multiple states, and some states have multiple national parks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please export this as an excel file that I can download to my computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChatGPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I apologize, as a language model, I am not able to directly create or export files. However, you can easily copy the table I provided and paste it into a new Excel document. To do this, simply follow these steps:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highlight the table (including the column headers and all rows of data)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right-click on the table and select "Copy" or use the keyboard shortcut "Ctrl + C"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open a new Excel document and click on the cell where you want to paste the table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right-click on the cell and select "Paste" or use the keyboard shortcut "Ctrl + V"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjust the formatting as desired.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I hope this helps!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Great Smoky Mountains National Park</t>
   </si>
   <si>
     <t xml:space="preserve">North Carolina, Tennessee</t>
   </si>
   <si>
-    <t xml:space="preserve"> { name: 'Great Smoky Mountains National Park', state: 'North Carolina, Tennessee' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guadalupe Mountains National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Guadalupe Mountains National Park', state: 'Texas' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haleakalā National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hawaii</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Haleakalā National Park', state: 'Hawaii' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hawai'i Volcanoes National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Hawai'i Volcanoes National Park', state: 'Hawaii' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hot Springs National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arkansas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Hot Springs National Park', state: 'Arkansas' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indiana Dunes National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Indiana Dunes National Park', state: 'Indiana' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isle Royale National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michigan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Isle Royale National Park', state: 'Michigan' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshua Tree National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Joshua Tree National Park', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katmai National Park and Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Katmai National Park and Preserve', state: 'Alaska' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenai Fjords National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Kenai Fjords National Park', state: 'Alaska' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kings Canyon National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Kings Canyon National Park', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kobuk Valley National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Kobuk Valley National Park', state: 'Alaska' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lake Clark National Park and Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Lake Clark National Park and Preserve', state: 'Alaska' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lassen Volcanic National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Lassen Volcanic National Park', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mammoth Cave National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kentucky</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Mammoth Cave National Park', state: 'Kentucky' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesa Verde National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Mesa Verde National Park', state: 'Colorado' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mount Rainier National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Washington</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Mount Rainier National Park', state: 'Washington' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Cascades National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'North Cascades National Park', state: 'Washington' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olympic National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Olympic National Park', state: 'Washington' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petrified Forest National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Petrified Forest National Park', state: 'Arizona' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinnacles National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Pinnacles National Park', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redwood National and State Parks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Redwood National and State Parks', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rocky Mountain National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Rocky Mountain National Park', state: 'Colorado' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saguaro National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Saguaro National Park', state: 'Arizona' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequoia National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Sequoia National Park', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shenandoah National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virginia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Shenandoah National Park', state: 'Virginia' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theodore Roosevelt National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Dakota</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Theodore Roosevelt National Park', state: 'North Dakota' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virgin Islands National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U.S. Virgin Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Virgin Islands National Park', state: 'U.S. Virgin Islands' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voyageurs National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minnesota</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Voyageurs National Park', state: 'Minnesota' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind Cave National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Wind Cave National Park', state: 'South Dakota' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrangell–St. Elias National Park and Preserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Wrangell–St. Elias National Park and Preserve', state: 'Alaska' },</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yellowstone National Park</t>
   </si>
   <si>
     <t xml:space="preserve">Wyoming, Montana, Idaho</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Yellowstone National Park', state: 'Wyoming, Montana, Idaho' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yosemite National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Yosemite National Park', state: 'California' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zion National Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> { name: 'Zion National Park', state: 'Utah' },</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note that some national parks span multiple states, and some states have multiple national parks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please export this as an excel file that I can download to my computer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChatGPT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I apologize, as a language model, I am not able to directly create or export files. However, you can easily copy the table I provided and paste it into a new Excel document. To do this, simply follow these steps:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highlight the table (including the column headers and all rows of data)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right-click on the table and select "Copy" or use the keyboard shortcut "Ctrl + C"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open a new Excel document and click on the cell where you want to paste the table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right-click on the cell and select "Paste" or use the keyboard shortcut "Ctrl + V"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adjust the formatting as desired.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I hope this helps!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code</t>
   </si>
 </sst>
 </file>
@@ -597,7 +639,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,8 +648,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFDBB6"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -645,12 +699,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,7 +743,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -731,18 +793,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J81"/>
+  <dimension ref="A2:M84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="43.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="43.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="26.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="66.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="63.89"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,1541 +812,1628 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A5&amp;B5&amp;C5&amp;D5&amp;E5)</f>
         <v> { name: 'Acadia National Park', state: 'Maine' },</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A6&amp;B6&amp;C6&amp;D6&amp;E6)</f>
-        <v> { name: 'American Samoa National Park', state: 'American Samoa' },</v>
+        <v>{ name: 'American Samoa National Park', state: 'American Samoa' },</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A7&amp;B7&amp;C7&amp;D7&amp;E7)</f>
-        <v> { name: 'Arches National Park', state: 'Utah' },</v>
+        <v>{ name: 'Arches National Park', state: 'Utah' },</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A8&amp;B8&amp;C8&amp;D8&amp;E8)</f>
-        <v> { name: 'Badlands National Park', state: 'South Dakota' },</v>
+        <v>{ name: 'Badlands National Park', state: 'South Dakota' },</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A9&amp;B9&amp;C9&amp;D9&amp;E9)</f>
-        <v> { name: 'Big Bend National Park', state: 'Texas' },</v>
+        <v>{ name: 'Big Bend National Park', state: 'Texas' },</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A10&amp;B10&amp;C10&amp;D10&amp;E10)</f>
-        <v> { name: 'Biscayne National Park', state: 'Florida' },</v>
+        <v>{ name: 'Biscayne National Park', state: 'Florida' },</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A11&amp;B11&amp;C11&amp;D11&amp;E11)</f>
-        <v> { name: 'Black Canyon of the Gunnison National Park', state: 'Colorado' },</v>
+        <v>{ name: 'Black Canyon of the Gunnison National Park', state: 'Colorado' },</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A12&amp;B12&amp;C12&amp;D12&amp;E12)</f>
-        <v> { name: 'Bryce Canyon National Park', state: 'Utah' },</v>
+        <v>{ name: 'Bryce Canyon National Park', state: 'Utah' },</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A13&amp;B13&amp;C13&amp;D13&amp;E13)</f>
-        <v> { name: 'Canyonlands National Park', state: 'Utah' },</v>
+        <v>{ name: 'Canyonlands National Park', state: 'Utah' },</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A14&amp;B14&amp;C14&amp;D14&amp;E14)</f>
-        <v> { name: 'Capitol Reef National Park', state: 'Utah' },</v>
+        <v>{ name: 'Capitol Reef National Park', state: 'Utah' },</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A15&amp;B15&amp;C15&amp;D15&amp;E15)</f>
-        <v> { name: 'Carlsbad Caverns National Park', state: 'New Mexico' },</v>
+        <v>{ name: 'Carlsbad Caverns National Park', state: 'New Mexico' },</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A16&amp;B16&amp;C16&amp;D16&amp;E16)</f>
-        <v> { name: 'Channel Islands National Park', state: 'California' },</v>
+        <v>{ name: 'Channel Islands National Park', state: 'California' },</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A17&amp;B17&amp;C17&amp;D17&amp;E17)</f>
-        <v> { name: 'Congaree National Park', state: 'South Carolina' },</v>
+        <v>{ name: 'Congaree National Park', state: 'South Carolina' },</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A18&amp;B18&amp;C18&amp;D18&amp;E18)</f>
-        <v> { name: 'Crater Lake National Park', state: 'Oregon' },</v>
+        <v>{ name: 'Crater Lake National Park', state: 'Oregon' },</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A19&amp;B19&amp;C19&amp;D19&amp;E19)</f>
-        <v> { name: 'Cuyahoga Valley National Park', state: 'Ohio' },</v>
+        <v>{ name: 'Cuyahoga Valley National Park', state: 'Ohio' },</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>60</v>
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A20&amp;B20&amp;C20&amp;D20&amp;E20)</f>
-        <v> { name: 'Death Valley National Park', state: 'California, Nevada' },</v>
+        <v>{ name: 'Death Valley National Park', state: 'California, Nevada' },</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A21&amp;B21&amp;C21&amp;D21&amp;E21)</f>
-        <v> { name: 'Denali National Park and Preserve', state: 'Alaska' },</v>
+        <v>{ name: 'Denali National Park and Preserve', state: 'Alaska' },</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A22&amp;B22&amp;C22&amp;D22&amp;E22)</f>
-        <v> { name: 'Dry Tortugas National Park', state: 'Florida' },</v>
+        <v>{ name: 'Dry Tortugas National Park', state: 'Florida' },</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A23&amp;B23&amp;C23&amp;D23&amp;E23)</f>
-        <v> { name: 'Everglades National Park', state: 'Florida' },</v>
+        <v>{ name: 'Everglades National Park', state: 'Florida' },</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A24&amp;B24&amp;C24&amp;D24&amp;E24)</f>
-        <v> { name: 'Gates of the Arctic National Park and Preserve', state: 'Alaska' },</v>
+        <v>{ name: 'Gates of the Arctic National Park and Preserve', state: 'Alaska' },</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A25&amp;B25&amp;C25&amp;D25&amp;E25)</f>
-        <v> { name: 'Glacier Bay National Park and Preserve', state: 'Alaska' },</v>
+        <v>{ name: 'Glacier Bay National Park and Preserve', state: 'Alaska' },</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A26&amp;B26&amp;C26&amp;D26&amp;E26)</f>
-        <v> { name: 'Glacier National Park', state: 'Montana' },</v>
+        <v>{ name: 'Glacier National Park', state: 'Montana' },</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A27&amp;B27&amp;C27&amp;D27&amp;E27)</f>
-        <v> { name: 'Grand Canyon National Park', state: 'Arizona' },</v>
+        <v>{ name: 'Grand Canyon National Park', state: 'Arizona' },</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A28&amp;B28&amp;C28&amp;D28&amp;E28)</f>
-        <v> { name: 'Grand Teton National Park', state: 'Wyoming' },</v>
+        <v>{ name: 'Grand Teton National Park', state: 'Wyoming' },</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A29&amp;B29&amp;C29&amp;D29&amp;E29)</f>
-        <v> { name: 'Great Basin National Park', state: 'Nevada' },</v>
+        <v>{ name: 'Great Basin National Park', state: 'Nevada' },</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A30&amp;B30&amp;C30&amp;D30&amp;E30)</f>
-        <v> { name: 'Great Sand Dunes National Park and Preserve', state: 'Colorado' },</v>
+        <v>{ name: 'Great Sand Dunes National Park and Preserve', state: 'Colorado' },</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>88</v>
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="0" t="str">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(A31&amp;B31&amp;C31&amp;D31&amp;E31)</f>
-        <v> { name: 'Great Smoky Mountains National Park', state: 'North Carolina, Tennessee' },</v>
+        <v> { name: 'Great Smoky Mountains National Park NC', state: 'North Carolina' },</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="0" t="str">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(A32&amp;B32&amp;C32&amp;D32&amp;E32)</f>
-        <v> { name: 'Guadalupe Mountains National Park', state: 'Texas' },</v>
+        <v> { name: 'Great Smoky Mountains National Park TN', state: 'Tennessee' },</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A33&amp;B33&amp;C33&amp;D33&amp;E33)</f>
-        <v> { name: 'Haleakalā National Park', state: 'Hawaii' },</v>
+        <v> { name: 'Guadalupe Mountains National Park', state: 'Texas' },</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A34&amp;B34&amp;C34&amp;D34&amp;E34)</f>
-        <v> { name: 'Hawai'i Volcanoes National Park', state: 'Hawaii' },</v>
+        <v>{ name: 'Haleakalā National Park', state: 'Hawaii' },</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A35&amp;B35&amp;C35&amp;D35&amp;E35)</f>
-        <v> { name: 'Hot Springs National Park', state: 'Arkansas' },</v>
+        <v>{ name: 'Hawai'i Volcanoes National Park', state: 'Hawaii' },</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A36&amp;B36&amp;C36&amp;D36&amp;E36)</f>
-        <v> { name: 'Indiana Dunes National Park', state: 'Indiana' },</v>
+        <v>{ name: 'Hot Springs National Park', state: 'Arkansas' },</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A37&amp;B37&amp;C37&amp;D37&amp;E37)</f>
-        <v> { name: 'Isle Royale National Park', state: 'Michigan' },</v>
+        <v>{ name: 'Indiana Dunes National Park', state: 'Indiana' },</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A38&amp;B38&amp;C38&amp;D38&amp;E38)</f>
-        <v> { name: 'Joshua Tree National Park', state: 'California' },</v>
+        <v>{ name: 'Isle Royale National Park', state: 'Michigan' },</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A39&amp;B39&amp;C39&amp;D39&amp;E39)</f>
-        <v> { name: 'Katmai National Park and Preserve', state: 'Alaska' },</v>
+        <v>{ name: 'Joshua Tree National Park', state: 'California' },</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A40&amp;B40&amp;C40&amp;D40&amp;E40)</f>
-        <v> { name: 'Kenai Fjords National Park', state: 'Alaska' },</v>
+        <v>{ name: 'Katmai National Park and Preserve', state: 'Alaska' },</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A41&amp;B41&amp;C41&amp;D41&amp;E41)</f>
-        <v> { name: 'Kings Canyon National Park', state: 'California' },</v>
+        <v>{ name: 'Kenai Fjords National Park', state: 'Alaska' },</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A42&amp;B42&amp;C42&amp;D42&amp;E42)</f>
-        <v> { name: 'Kobuk Valley National Park', state: 'Alaska' },</v>
+        <v>{ name: 'Kings Canyon National Park', state: 'California' },</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A43&amp;B43&amp;C43&amp;D43&amp;E43)</f>
-        <v> { name: 'Lake Clark National Park and Preserve', state: 'Alaska' },</v>
+        <v>{ name: 'Kobuk Valley National Park', state: 'Alaska' },</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A44&amp;B44&amp;C44&amp;D44&amp;E44)</f>
-        <v> { name: 'Lassen Volcanic National Park', state: 'California' },</v>
+        <v>{ name: 'Lake Clark National Park and Preserve', state: 'Alaska' },</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A45&amp;B45&amp;C45&amp;D45&amp;E45)</f>
-        <v> { name: 'Mammoth Cave National Park', state: 'Kentucky' },</v>
+        <v>{ name: 'Lassen Volcanic National Park', state: 'California' },</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A46&amp;B46&amp;C46&amp;D46&amp;E46)</f>
-        <v> { name: 'Mesa Verde National Park', state: 'Colorado' },</v>
+        <v>{ name: 'Mammoth Cave National Park', state: 'Kentucky' },</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>126</v>
+        <v>35</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A47&amp;B47&amp;C47&amp;D47&amp;E47)</f>
-        <v> { name: 'Mount Rainier National Park', state: 'Washington' },</v>
+        <v>{ name: 'Mesa Verde National Park', state: 'Colorado' },</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A48&amp;B48&amp;C48&amp;D48&amp;E48)</f>
-        <v> { name: 'North Cascades National Park', state: 'Washington' },</v>
+        <v>{ name: 'Mount Rainier National Park', state: 'Washington' },</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A49&amp;B49&amp;C49&amp;D49&amp;E49)</f>
-        <v> { name: 'Olympic National Park', state: 'Washington' },</v>
+        <v>{ name: 'North Cascades National Park', state: 'Washington' },</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="E50" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A50&amp;B50&amp;C50&amp;D50&amp;E50)</f>
-        <v> { name: 'Petrified Forest National Park', state: 'Arizona' },</v>
+        <v>{ name: 'Olympic National Park', state: 'Washington' },</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A51&amp;B51&amp;C51&amp;D51&amp;E51)</f>
-        <v> { name: 'Pinnacles National Park', state: 'California' },</v>
+        <v>{ name: 'Petrified Forest National Park', state: 'Arizona' },</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A52&amp;B52&amp;C52&amp;D52&amp;E52)</f>
-        <v> { name: 'Redwood National and State Parks', state: 'California' },</v>
+        <v>{ name: 'Pinnacles National Park', state: 'California' },</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A53&amp;B53&amp;C53&amp;D53&amp;E53)</f>
-        <v> { name: 'Rocky Mountain National Park', state: 'Colorado' },</v>
+        <v>{ name: 'Redwood National and State Parks', state: 'California' },</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A54&amp;B54&amp;C54&amp;D54&amp;E54)</f>
-        <v> { name: 'Saguaro National Park', state: 'Arizona' },</v>
+        <v>{ name: 'Rocky Mountain National Park', state: 'Colorado' },</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A55&amp;B55&amp;C55&amp;D55&amp;E55)</f>
-        <v> { name: 'Sequoia National Park', state: 'California' },</v>
+        <v>{ name: 'Saguaro National Park', state: 'Arizona' },</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A56&amp;B56&amp;C56&amp;D56&amp;E56)</f>
-        <v> { name: 'Shenandoah National Park', state: 'Virginia' },</v>
+        <v>{ name: 'Sequoia National Park', state: 'California' },</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A57&amp;B57&amp;C57&amp;D57&amp;E57)</f>
-        <v> { name: 'Theodore Roosevelt National Park', state: 'North Dakota' },</v>
+        <v>{ name: 'Shenandoah National Park', state: 'Virginia' },</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A58&amp;B58&amp;C58&amp;D58&amp;E58)</f>
-        <v> { name: 'Virgin Islands National Park', state: 'U.S. Virgin Islands' },</v>
+        <v>{ name: 'Theodore Roosevelt National Park', state: 'North Dakota' },</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A59&amp;B59&amp;C59&amp;D59&amp;E59)</f>
-        <v> { name: 'Voyageurs National Park', state: 'Minnesota' },</v>
+        <v>{ name: 'Virgin Islands National Park', state: 'U.S. Virgin Islands' },</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A60&amp;B60&amp;C60&amp;D60&amp;E60)</f>
-        <v> { name: 'Wind Cave National Park', state: 'South Dakota' },</v>
+        <v>{ name: 'Voyageurs National Park', state: 'Minnesota' },</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A61&amp;B61&amp;C61&amp;D61&amp;E61)</f>
-        <v> { name: 'Wrangell–St. Elias National Park and Preserve', state: 'Alaska' },</v>
+        <v>{ name: 'Wind Cave National Park', state: 'South Dakota' },</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>161</v>
+        <v>66</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A62&amp;B62&amp;C62&amp;D62&amp;E62)</f>
-        <v> { name: 'Yellowstone National Park', state: 'Wyoming, Montana, Idaho' },</v>
+        <v>{ name: 'Wrangell–St. Elias National Park and Preserve', state: 'Alaska' },</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A63&amp;B63&amp;C63&amp;D63&amp;E63)</f>
-        <v> { name: 'Yosemite National Park', state: 'California' },</v>
+        <v> { name: 'Yellowstone National Park ID', state: 'Idaho' },</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A64&amp;B64&amp;C64&amp;D64&amp;E64)</f>
+        <v> { name: 'Yellowstone National Park MT', state: 'Montana' },</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A65&amp;B65&amp;C65&amp;D65&amp;E65)</f>
+        <v> { name: 'Yellowstone National Park WY', state: 'Wyoming' },</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A66&amp;B66&amp;C66&amp;D66&amp;E66)</f>
+        <v>{ name: 'Yosemite National Park', state: 'California' },</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(A67&amp;B67&amp;C67&amp;D67&amp;E67)</f>
         <v> { name: 'Zion National Park', state: 'Utah' },</v>
       </c>
-      <c r="G64" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
-        <v>170</v>
+      <c r="G67" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>171</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>177</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2309,38 +2458,38 @@
       <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.97"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="D4" s="0" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G5" s="0" t="e">
         <f aca="false">concatanate(D5 &amp; A5 &amp; E5 &amp; F5)</f>
@@ -2349,562 +2498,562 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>